<commit_message>
Randimize row order to make it work on logistic analysis model evaluation
</commit_message>
<xml_diff>
--- a/docs/analysis/data/mtcars.xlsx
+++ b/docs/analysis/data/mtcars.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amo.QTSEL\Documents\Qlik\Sense\Extensions\advanced-analytics-toolbox\docs\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Masaki Hamano\Documents\Qlik\Sense\Extensions\advanced-analytics-toolbox\docs\analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -552,7 +552,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -609,7 +611,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>21</v>
@@ -627,10 +629,10 @@
         <v>3.9</v>
       </c>
       <c r="G2">
-        <v>2.62</v>
+        <v>2.875</v>
       </c>
       <c r="H2">
-        <v>16.46</v>
+        <v>17.02</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -647,7 +649,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>21</v>
@@ -665,10 +667,10 @@
         <v>3.9</v>
       </c>
       <c r="G3">
-        <v>2.875</v>
+        <v>2.62</v>
       </c>
       <c r="H3">
-        <v>17.02</v>
+        <v>16.46</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -685,145 +687,145 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="B4">
-        <v>22.8</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D4">
-        <v>108</v>
+        <v>301</v>
       </c>
       <c r="E4">
-        <v>93</v>
+        <v>335</v>
       </c>
       <c r="F4">
-        <v>3.85</v>
+        <v>3.54</v>
       </c>
       <c r="G4">
-        <v>2.3199999999999998</v>
+        <v>3.57</v>
       </c>
       <c r="H4">
-        <v>18.61</v>
+        <v>14.6</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
       <c r="K4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="B5">
-        <v>21.4</v>
+        <v>30.4</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>258</v>
+        <v>95.1</v>
       </c>
       <c r="E5">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F5">
-        <v>3.08</v>
+        <v>3.77</v>
       </c>
       <c r="G5">
-        <v>3.2149999999999999</v>
+        <v>1.5129999999999999</v>
       </c>
       <c r="H5">
-        <v>19.440000000000001</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="B6">
-        <v>18.7</v>
+        <v>19.7</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6">
-        <v>360</v>
+        <v>145</v>
       </c>
       <c r="E6">
         <v>175</v>
       </c>
       <c r="F6">
-        <v>3.15</v>
+        <v>3.62</v>
       </c>
       <c r="G6">
-        <v>3.44</v>
+        <v>2.77</v>
       </c>
       <c r="H6">
-        <v>17.02</v>
+        <v>15.5</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L6">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7">
-        <v>18.100000000000001</v>
+        <v>18.7</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D7">
-        <v>225</v>
+        <v>360</v>
       </c>
       <c r="E7">
-        <v>105</v>
+        <v>175</v>
       </c>
       <c r="F7">
-        <v>2.76</v>
+        <v>3.15</v>
       </c>
       <c r="G7">
-        <v>3.46</v>
+        <v>3.44</v>
       </c>
       <c r="H7">
-        <v>20.22</v>
+        <v>17.02</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -832,33 +834,33 @@
         <v>3</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B8">
-        <v>14.3</v>
+        <v>17.3</v>
       </c>
       <c r="C8">
         <v>8</v>
       </c>
       <c r="D8">
-        <v>360</v>
+        <v>275.8</v>
       </c>
       <c r="E8">
-        <v>245</v>
+        <v>180</v>
       </c>
       <c r="F8">
-        <v>3.21</v>
+        <v>3.07</v>
       </c>
       <c r="G8">
-        <v>3.57</v>
+        <v>3.73</v>
       </c>
       <c r="H8">
-        <v>15.84</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -870,71 +872,71 @@
         <v>3</v>
       </c>
       <c r="L8">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B9">
-        <v>24.4</v>
+        <v>10.4</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D9">
-        <v>146.69999999999999</v>
+        <v>472</v>
       </c>
       <c r="E9">
-        <v>62</v>
+        <v>205</v>
       </c>
       <c r="F9">
-        <v>3.69</v>
+        <v>2.93</v>
       </c>
       <c r="G9">
-        <v>3.19</v>
+        <v>5.25</v>
       </c>
       <c r="H9">
-        <v>20</v>
+        <v>17.98</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L9">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10">
-        <v>22.8</v>
+        <v>19.2</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D10">
-        <v>140.80000000000001</v>
+        <v>167.6</v>
       </c>
       <c r="E10">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="F10">
         <v>3.92</v>
       </c>
       <c r="G10">
-        <v>3.15</v>
+        <v>3.44</v>
       </c>
       <c r="H10">
-        <v>22.9</v>
+        <v>18.3</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -946,80 +948,80 @@
         <v>4</v>
       </c>
       <c r="L10">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B11">
-        <v>19.2</v>
+        <v>27.3</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D11">
-        <v>167.6</v>
+        <v>79</v>
       </c>
       <c r="E11">
-        <v>123</v>
+        <v>66</v>
       </c>
       <c r="F11">
-        <v>3.92</v>
+        <v>4.08</v>
       </c>
       <c r="G11">
-        <v>3.44</v>
+        <v>1.9350000000000001</v>
       </c>
       <c r="H11">
-        <v>18.3</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="I11">
         <v>1</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11">
         <v>4</v>
       </c>
       <c r="L11">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B12">
-        <v>17.8</v>
+        <v>13.3</v>
       </c>
       <c r="C12">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D12">
-        <v>167.6</v>
+        <v>350</v>
       </c>
       <c r="E12">
-        <v>123</v>
+        <v>245</v>
       </c>
       <c r="F12">
-        <v>3.92</v>
+        <v>3.73</v>
       </c>
       <c r="G12">
-        <v>3.44</v>
+        <v>3.84</v>
       </c>
       <c r="H12">
-        <v>18.899999999999999</v>
+        <v>15.41</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12">
         <v>0</v>
       </c>
       <c r="K12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L12">
         <v>4</v>
@@ -1027,66 +1029,66 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B13">
-        <v>16.399999999999999</v>
+        <v>26</v>
       </c>
       <c r="C13">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D13">
-        <v>275.8</v>
+        <v>120.3</v>
       </c>
       <c r="E13">
-        <v>180</v>
+        <v>91</v>
       </c>
       <c r="F13">
-        <v>3.07</v>
+        <v>4.43</v>
       </c>
       <c r="G13">
-        <v>4.07</v>
+        <v>2.14</v>
       </c>
       <c r="H13">
-        <v>17.399999999999999</v>
+        <v>16.7</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L13">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B14">
-        <v>17.3</v>
+        <v>15.5</v>
       </c>
       <c r="C14">
         <v>8</v>
       </c>
       <c r="D14">
-        <v>275.8</v>
+        <v>318</v>
       </c>
       <c r="E14">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="F14">
-        <v>3.07</v>
+        <v>2.76</v>
       </c>
       <c r="G14">
-        <v>3.73</v>
+        <v>3.52</v>
       </c>
       <c r="H14">
-        <v>17.600000000000001</v>
+        <v>16.87</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -1098,33 +1100,33 @@
         <v>3</v>
       </c>
       <c r="L14">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B15">
-        <v>15.2</v>
+        <v>19.2</v>
       </c>
       <c r="C15">
         <v>8</v>
       </c>
       <c r="D15">
-        <v>275.8</v>
+        <v>400</v>
       </c>
       <c r="E15">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F15">
-        <v>3.07</v>
+        <v>3.08</v>
       </c>
       <c r="G15">
-        <v>3.78</v>
+        <v>3.8450000000000002</v>
       </c>
       <c r="H15">
-        <v>18</v>
+        <v>17.05</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -1136,156 +1138,156 @@
         <v>3</v>
       </c>
       <c r="L15">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B16">
-        <v>10.4</v>
+        <v>30.4</v>
       </c>
       <c r="C16">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D16">
-        <v>472</v>
+        <v>75.7</v>
       </c>
       <c r="E16">
-        <v>205</v>
+        <v>52</v>
       </c>
       <c r="F16">
-        <v>2.93</v>
+        <v>4.93</v>
       </c>
       <c r="G16">
-        <v>5.25</v>
+        <v>1.615</v>
       </c>
       <c r="H16">
-        <v>17.98</v>
+        <v>18.52</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L16">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B17">
-        <v>10.4</v>
+        <v>24.4</v>
       </c>
       <c r="C17">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D17">
-        <v>460</v>
+        <v>146.69999999999999</v>
       </c>
       <c r="E17">
-        <v>215</v>
+        <v>62</v>
       </c>
       <c r="F17">
-        <v>3</v>
+        <v>3.69</v>
       </c>
       <c r="G17">
-        <v>5.4240000000000004</v>
+        <v>3.19</v>
       </c>
       <c r="H17">
-        <v>17.82</v>
+        <v>20</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17">
         <v>0</v>
       </c>
       <c r="K17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L17">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18">
-        <v>14.7</v>
+        <v>32.4</v>
       </c>
       <c r="C18">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D18">
-        <v>440</v>
+        <v>78.7</v>
       </c>
       <c r="E18">
-        <v>230</v>
+        <v>66</v>
       </c>
       <c r="F18">
-        <v>3.23</v>
+        <v>4.08</v>
       </c>
       <c r="G18">
-        <v>5.3449999999999998</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H18">
-        <v>17.420000000000002</v>
+        <v>19.47</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L18">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B19">
-        <v>32.4</v>
+        <v>21.4</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D19">
-        <v>78.7</v>
+        <v>258</v>
       </c>
       <c r="E19">
-        <v>66</v>
+        <v>110</v>
       </c>
       <c r="F19">
-        <v>4.08</v>
+        <v>3.08</v>
       </c>
       <c r="G19">
-        <v>2.2000000000000002</v>
+        <v>3.2149999999999999</v>
       </c>
       <c r="H19">
-        <v>19.47</v>
+        <v>19.440000000000001</v>
       </c>
       <c r="I19">
         <v>1</v>
       </c>
       <c r="J19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L19">
         <v>1</v>
@@ -1293,40 +1295,40 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B20">
-        <v>30.4</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D20">
-        <v>75.7</v>
+        <v>275.8</v>
       </c>
       <c r="E20">
-        <v>52</v>
+        <v>180</v>
       </c>
       <c r="F20">
-        <v>4.93</v>
+        <v>3.07</v>
       </c>
       <c r="G20">
-        <v>1.615</v>
+        <v>4.07</v>
       </c>
       <c r="H20">
-        <v>18.52</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="I20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L20">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.4">
@@ -1407,28 +1409,28 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B23">
-        <v>15.5</v>
+        <v>15.2</v>
       </c>
       <c r="C23">
         <v>8</v>
       </c>
       <c r="D23">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="E23">
         <v>150</v>
       </c>
       <c r="F23">
-        <v>2.76</v>
+        <v>3.15</v>
       </c>
       <c r="G23">
-        <v>3.52</v>
+        <v>3.4350000000000001</v>
       </c>
       <c r="H23">
-        <v>16.87</v>
+        <v>17.3</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -1445,31 +1447,31 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="B24">
-        <v>15.2</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="C24">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D24">
-        <v>304</v>
+        <v>225</v>
       </c>
       <c r="E24">
-        <v>150</v>
+        <v>105</v>
       </c>
       <c r="F24">
-        <v>3.15</v>
+        <v>2.76</v>
       </c>
       <c r="G24">
-        <v>3.4350000000000001</v>
+        <v>3.46</v>
       </c>
       <c r="H24">
-        <v>17.3</v>
+        <v>20.22</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24">
         <v>0</v>
@@ -1478,42 +1480,42 @@
         <v>3</v>
       </c>
       <c r="L24">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B25">
-        <v>13.3</v>
+        <v>15.8</v>
       </c>
       <c r="C25">
         <v>8</v>
       </c>
       <c r="D25">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E25">
-        <v>245</v>
+        <v>264</v>
       </c>
       <c r="F25">
-        <v>3.73</v>
+        <v>4.22</v>
       </c>
       <c r="G25">
-        <v>3.84</v>
+        <v>3.17</v>
       </c>
       <c r="H25">
-        <v>15.41</v>
+        <v>14.5</v>
       </c>
       <c r="I25">
         <v>0</v>
       </c>
       <c r="J25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L25">
         <v>4</v>
@@ -1521,28 +1523,28 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B26">
-        <v>19.2</v>
+        <v>14.7</v>
       </c>
       <c r="C26">
         <v>8</v>
       </c>
       <c r="D26">
-        <v>400</v>
+        <v>440</v>
       </c>
       <c r="E26">
-        <v>175</v>
+        <v>230</v>
       </c>
       <c r="F26">
-        <v>3.08</v>
+        <v>3.23</v>
       </c>
       <c r="G26">
-        <v>3.8450000000000002</v>
+        <v>5.3449999999999998</v>
       </c>
       <c r="H26">
-        <v>17.05</v>
+        <v>17.420000000000002</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -1554,33 +1556,33 @@
         <v>3</v>
       </c>
       <c r="L26">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B27">
-        <v>27.3</v>
+        <v>21.4</v>
       </c>
       <c r="C27">
         <v>4</v>
       </c>
       <c r="D27">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="E27">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="F27">
-        <v>4.08</v>
+        <v>4.1100000000000003</v>
       </c>
       <c r="G27">
-        <v>1.9350000000000001</v>
+        <v>2.78</v>
       </c>
       <c r="H27">
-        <v>18.899999999999999</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="I27">
         <v>1</v>
@@ -1592,118 +1594,118 @@
         <v>4</v>
       </c>
       <c r="L27">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B28">
-        <v>26</v>
+        <v>17.8</v>
       </c>
       <c r="C28">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D28">
-        <v>120.3</v>
+        <v>167.6</v>
       </c>
       <c r="E28">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="F28">
-        <v>4.43</v>
+        <v>3.92</v>
       </c>
       <c r="G28">
-        <v>2.14</v>
+        <v>3.44</v>
       </c>
       <c r="H28">
-        <v>16.7</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L28">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B29">
-        <v>30.4</v>
+        <v>10.4</v>
       </c>
       <c r="C29">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D29">
-        <v>95.1</v>
+        <v>460</v>
       </c>
       <c r="E29">
-        <v>113</v>
+        <v>215</v>
       </c>
       <c r="F29">
-        <v>3.77</v>
+        <v>3</v>
       </c>
       <c r="G29">
-        <v>1.5129999999999999</v>
+        <v>5.4240000000000004</v>
       </c>
       <c r="H29">
-        <v>16.899999999999999</v>
+        <v>17.82</v>
       </c>
       <c r="I29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K29">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L29">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="B30">
-        <v>15.8</v>
+        <v>14.3</v>
       </c>
       <c r="C30">
         <v>8</v>
       </c>
       <c r="D30">
-        <v>351</v>
+        <v>360</v>
       </c>
       <c r="E30">
-        <v>264</v>
+        <v>245</v>
       </c>
       <c r="F30">
-        <v>4.22</v>
+        <v>3.21</v>
       </c>
       <c r="G30">
-        <v>3.17</v>
+        <v>3.57</v>
       </c>
       <c r="H30">
-        <v>14.5</v>
+        <v>15.84</v>
       </c>
       <c r="I30">
         <v>0</v>
       </c>
       <c r="J30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K30">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L30">
         <v>4</v>
@@ -1711,104 +1713,104 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B31">
-        <v>19.7</v>
+        <v>15.2</v>
       </c>
       <c r="C31">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D31">
-        <v>145</v>
+        <v>275.8</v>
       </c>
       <c r="E31">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="F31">
-        <v>3.62</v>
+        <v>3.07</v>
       </c>
       <c r="G31">
-        <v>2.77</v>
+        <v>3.78</v>
       </c>
       <c r="H31">
-        <v>15.5</v>
+        <v>18</v>
       </c>
       <c r="I31">
         <v>0</v>
       </c>
       <c r="J31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K31">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L31">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="B32">
-        <v>15</v>
+        <v>22.8</v>
       </c>
       <c r="C32">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D32">
-        <v>301</v>
+        <v>140.80000000000001</v>
       </c>
       <c r="E32">
-        <v>335</v>
+        <v>95</v>
       </c>
       <c r="F32">
-        <v>3.54</v>
+        <v>3.92</v>
       </c>
       <c r="G32">
-        <v>3.57</v>
+        <v>3.15</v>
       </c>
       <c r="H32">
-        <v>14.6</v>
+        <v>22.9</v>
       </c>
       <c r="I32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K32">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L32">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B33">
-        <v>21.4</v>
+        <v>22.8</v>
       </c>
       <c r="C33">
         <v>4</v>
       </c>
       <c r="D33">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="E33">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="F33">
-        <v>4.1100000000000003</v>
+        <v>3.85</v>
       </c>
       <c r="G33">
-        <v>2.78</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="H33">
-        <v>18.600000000000001</v>
+        <v>18.61</v>
       </c>
       <c r="I33">
         <v>1</v>
@@ -1820,7 +1822,7 @@
         <v>4</v>
       </c>
       <c r="L33">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>